<commit_message>
add models of order details
</commit_message>
<xml_diff>
--- a/Designing prices in - product Deatisl.xlsx
+++ b/Designing prices in - product Deatisl.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="11020"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
   <si>
     <t>INTAGLI CAD SOLUTIONS (By Confident Dental Laboratory Pvt Ltd)</t>
   </si>
@@ -179,22 +182,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -204,13 +194,13 @@
       <name val="Arial Black"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="16"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -255,55 +245,44 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -313,24 +292,77 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -532,7 +564,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -550,7 +582,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -579,7 +611,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -604,7 +636,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -629,7 +661,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -654,7 +686,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -679,7 +711,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -704,7 +736,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -729,7 +761,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -754,7 +786,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -779,7 +811,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -792,9 +824,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -811,7 +849,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -829,7 +867,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -854,7 +892,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -879,7 +917,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -904,7 +942,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -929,7 +967,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -954,7 +992,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,7 +1017,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1004,7 +1042,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1029,7 +1067,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1054,7 +1092,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1067,9 +1105,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1083,7 +1127,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1101,7 +1145,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1130,7 +1174,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1155,7 +1199,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1180,7 +1224,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1205,7 +1249,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1230,7 +1274,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1255,7 +1299,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1280,7 +1324,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1305,7 +1349,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1330,7 +1374,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1343,563 +1387,573 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="53.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="24" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45.75" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:6" ht="45.75" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" ht="24.75" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" t="s" s="6">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="24.75" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" ht="24.75" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" t="s" s="6">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="24.75" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" ht="21" customHeight="1">
-      <c r="A4" t="s" s="8">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="21" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s" s="8">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s" s="8">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s" s="8">
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s" s="9">
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="10">
+    <row r="5" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" t="s" s="11">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s" s="11">
+      <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s" s="11">
+      <c r="F5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="10">
+    <row r="6" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" t="s" s="11">
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s" s="11">
+      <c r="C6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s" s="11">
+      <c r="D6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s" s="11">
+      <c r="E6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s" s="11">
+      <c r="F6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="10">
+    <row r="7" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" t="s" s="11">
+      <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s" s="11">
+      <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s" s="11">
+      <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s" s="11">
+      <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s" s="11">
+      <c r="F7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="10">
+    <row r="8" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" t="s" s="11">
+      <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s" s="11">
+      <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s" s="11">
+      <c r="D8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s" s="11">
+      <c r="E8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F8" t="s" s="11">
+      <c r="F8" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="10">
+    <row r="9" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" t="s" s="11">
+      <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s" s="11">
+      <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" t="s" s="11">
+      <c r="D9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s" s="11">
+      <c r="E9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F9" t="s" s="11">
+      <c r="F9" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="10">
+    <row r="10" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B10" t="s" s="11">
+      <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s" s="11">
+      <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s" s="11">
+      <c r="D10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s" s="11">
+      <c r="E10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F10" t="s" s="11">
+      <c r="F10" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" ht="21" customHeight="1">
-      <c r="A11" t="s" s="8">
+    <row r="11" spans="1:6" ht="21" customHeight="1">
+      <c r="A11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="13">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A12" s="8">
         <v>1</v>
       </c>
-      <c r="B12" t="s" s="14">
+      <c r="B12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s" s="11">
+      <c r="C12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s" s="11">
+      <c r="D12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s" s="11">
+      <c r="E12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F12" t="s" s="11">
+      <c r="F12" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="13">
+    <row r="13" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A13" s="8">
         <v>2</v>
       </c>
-      <c r="B13" t="s" s="14">
+      <c r="B13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s" s="11">
+      <c r="C13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D13" t="s" s="11">
+      <c r="D13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E13" t="s" s="11">
+      <c r="E13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F13" t="s" s="11">
+      <c r="F13" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="13">
+    <row r="14" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A14" s="8">
         <v>3</v>
       </c>
-      <c r="B14" t="s" s="14">
+      <c r="B14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s" s="11">
+      <c r="C14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D14" t="s" s="11">
+      <c r="D14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E14" t="s" s="11">
+      <c r="E14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F14" t="s" s="11">
+      <c r="F14" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" s="13">
+    <row r="15" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A15" s="8">
         <v>4</v>
       </c>
-      <c r="B15" t="s" s="14">
+      <c r="B15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s" s="11">
+      <c r="C15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s" s="11">
+      <c r="D15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E15" t="s" s="11">
+      <c r="E15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F15" t="s" s="11">
+      <c r="F15" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" s="13">
+    <row r="16" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A16" s="8">
         <v>5</v>
       </c>
-      <c r="B16" t="s" s="14">
+      <c r="B16" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C16" t="s" s="11">
+      <c r="C16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D16" t="s" s="11">
+      <c r="D16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E16" t="s" s="11">
+      <c r="E16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F16" t="s" s="11">
+      <c r="F16" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" s="13">
+    <row r="17" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A17" s="8">
         <v>6</v>
       </c>
-      <c r="B17" t="s" s="14">
+      <c r="B17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C17" t="s" s="11">
+      <c r="C17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D17" t="s" s="11">
+      <c r="D17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E17" t="s" s="11">
+      <c r="E17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F17" t="s" s="11">
+      <c r="F17" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" s="13">
+    <row r="18" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A18" s="8">
         <v>7</v>
       </c>
-      <c r="B18" t="s" s="14">
+      <c r="B18" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C18" t="s" s="11">
+      <c r="C18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D18" t="s" s="11">
+      <c r="D18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E18" t="s" s="11">
+      <c r="E18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F18" t="s" s="11">
+      <c r="F18" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" ht="13.55" customHeight="1">
-      <c r="A19" s="13">
+    <row r="19" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A19" s="8">
         <v>8</v>
       </c>
-      <c r="B19" t="s" s="14">
+      <c r="B19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C19" t="s" s="11">
+      <c r="C19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D19" t="s" s="11">
+      <c r="D19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E19" t="s" s="11">
+      <c r="E19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F19" t="s" s="11">
+      <c r="F19" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" s="13">
+    <row r="20" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A20" s="8">
         <v>9</v>
       </c>
-      <c r="B20" t="s" s="14">
+      <c r="B20" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C20" t="s" s="11">
+      <c r="C20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="11">
+      <c r="D20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E20" t="s" s="11">
+      <c r="E20" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F20" t="s" s="11">
+      <c r="F20" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" ht="13.55" customHeight="1">
-      <c r="A21" s="13">
+    <row r="21" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A21" s="8">
         <v>10</v>
       </c>
-      <c r="B21" t="s" s="14">
+      <c r="B21" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C21" t="s" s="11">
+      <c r="C21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="11">
+      <c r="D21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E21" t="s" s="11">
+      <c r="E21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F21" t="s" s="11">
+      <c r="F21" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" s="13">
+    <row r="22" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A22" s="8">
         <v>11</v>
       </c>
-      <c r="B22" t="s" s="14">
+      <c r="B22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C22" t="s" s="11">
+      <c r="C22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D22" t="s" s="11">
+      <c r="D22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E22" t="s" s="11">
+      <c r="E22" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F22" t="s" s="11">
+      <c r="F22" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" s="13">
+    <row r="23" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A23" s="8">
         <v>12</v>
       </c>
-      <c r="B23" t="s" s="14">
+      <c r="B23" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C23" t="s" s="11">
+      <c r="C23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D23" t="s" s="11">
+      <c r="D23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E23" t="s" s="11">
+      <c r="E23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F23" t="s" s="11">
+      <c r="F23" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" ht="21" customHeight="1">
-      <c r="A24" t="s" s="8">
+    <row r="24" spans="1:6" ht="21" customHeight="1">
+      <c r="A24" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" ht="13.55" customHeight="1">
-      <c r="A25" s="13">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A25" s="8">
         <v>1</v>
       </c>
-      <c r="B25" t="s" s="14">
+      <c r="B25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C25" t="s" s="11">
+      <c r="C25" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D25" t="s" s="11">
+      <c r="D25" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E25" t="s" s="11">
+      <c r="E25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F25" t="s" s="11">
+      <c r="F25" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" ht="13.55" customHeight="1">
-      <c r="A26" s="13">
+    <row r="26" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A26" s="8">
         <v>2</v>
       </c>
-      <c r="B26" t="s" s="14">
+      <c r="B26" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C26" t="s" s="11">
+      <c r="C26" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D26" t="s" s="11">
+      <c r="D26" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E26" t="s" s="11">
+      <c r="E26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F26" t="s" s="11">
+      <c r="F26" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" ht="13.55" customHeight="1">
-      <c r="A27" s="13">
+    <row r="27" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A27" s="8">
         <v>3</v>
       </c>
-      <c r="B27" t="s" s="14">
+      <c r="B27" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C27" t="s" s="11">
+      <c r="C27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D27" t="s" s="11">
+      <c r="D27" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E27" t="s" s="11">
+      <c r="E27" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F27" t="s" s="11">
+      <c r="F27" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" ht="13.55" customHeight="1">
-      <c r="A28" s="13">
+    <row r="28" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A28" s="8">
         <v>4</v>
       </c>
-      <c r="B28" t="s" s="14">
+      <c r="B28" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C28" t="s" s="11">
+      <c r="C28" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D28" t="s" s="11">
+      <c r="D28" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E28" t="s" s="11">
+      <c r="E28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F28" t="s" s="11">
+      <c r="F28" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" ht="13.55" customHeight="1">
-      <c r="A29" s="13">
+    <row r="29" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A29" s="8">
         <v>5</v>
       </c>
-      <c r="B29" t="s" s="14">
+      <c r="B29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C29" t="s" s="11">
+      <c r="C29" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D29" t="s" s="11">
+      <c r="D29" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E29" t="s" s="11">
+      <c r="E29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F29" t="s" s="11">
+      <c r="F29" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1911,8 +1965,8 @@
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A24:D24"/>
   </mergeCells>
-  <pageMargins left="0.511811" right="0.511811" top="0.354331" bottom="0.354331" header="0.314961" footer="0.314961"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageMargins left="0.51181100000000002" right="0.51181100000000002" top="0.35433100000000001" bottom="0.35433100000000001" header="0.31496099999999999" footer="0.31496099999999999"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>